<commit_message>
quick tour v3 and login added
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="326">
   <si>
     <t xml:space="preserve">KEY</t>
   </si>
@@ -574,6 +574,21 @@
     <t xml:space="preserve">Commander</t>
   </si>
   <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passwort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parola d'accesso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mot de passe</t>
+  </si>
+  <si>
     <t xml:space="preserve">order-qr-payment</t>
   </si>
   <si>
@@ -920,6 +935,105 @@
   </si>
   <si>
     <t xml:space="preserve">Notificazioni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enter-username-pwd</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Please enter username </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'test' and password 'test'!</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Bitte Benutzername 'test' und Passwort 'test' eingeben!</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Pregasi immetere il nome dell utente </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'test' e la parola d‘accesso 'test'!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Entrez le nom d‘utilisateur </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'test' et le mot de passe 'test', s.v.p.!</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">start-the-tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start the tour…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beginne die Tour…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incomincia il giro…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commencez le tour…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benutzername</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome utente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom d'utilisateur</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -947,7 +1061,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -978,6 +1092,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1128,8 +1248,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
@@ -2443,7 +2563,7 @@
         <v>"order" : "Commander",</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>184</v>
       </c>
@@ -2461,22 +2581,22 @@
       </c>
       <c r="F41" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A41,""" : """,B41,""",")</f>
-        <v>"order-qr-payment" : "To order a QR payment, please provide account and amount!",</v>
+        <v>"password" : "Password",</v>
       </c>
       <c r="G41" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A41,""" : """,C41,""",")</f>
-        <v>"order-qr-payment" : "Konto und Betrag müssen ausgefüllt sein, damit eine QR-Zahlung bestellt werden kann!",</v>
+        <v>"password" : "Passwort",</v>
       </c>
       <c r="H41" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A41,""" : """,D41,""",")</f>
-        <v>"order-qr-payment" : "Si prega di mettere a disposizione il conto e il montante per potere ordinare il pagamento QR! ",</v>
+        <v>"password" : "Parola d'accesso",</v>
       </c>
       <c r="I41" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A41,""" : """,E41,""",")</f>
-        <v>"order-qr-payment" : "Compte et montant doivent être remplis avant de commander un paiement QR!",</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"password" : "Mot de passe",</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>189</v>
       </c>
@@ -2494,19 +2614,19 @@
       </c>
       <c r="F42" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A42,""" : """,B42,""",")</f>
-        <v>"qr-payment" : "QR Payment",</v>
+        <v>"order-qr-payment" : "To order a QR payment, please provide account and amount!",</v>
       </c>
       <c r="G42" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A42,""" : """,C42,""",")</f>
-        <v>"qr-payment" : "QR-Zahlung",</v>
+        <v>"order-qr-payment" : "Konto und Betrag müssen ausgefüllt sein, damit eine QR-Zahlung bestellt werden kann!",</v>
       </c>
       <c r="H42" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A42,""" : """,D42,""",")</f>
-        <v>"qr-payment" : "Pagamento QR",</v>
+        <v>"order-qr-payment" : "Si prega di mettere a disposizione il conto e il montante per potere ordinare il pagamento QR! ",</v>
       </c>
       <c r="I42" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A42,""" : """,E42,""",")</f>
-        <v>"qr-payment" : "Paiement QR",</v>
+        <v>"order-qr-payment" : "Compte et montant doivent être remplis avant de commander un paiement QR!",</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2527,19 +2647,19 @@
       </c>
       <c r="F43" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A43,""" : """,B43,""",")</f>
-        <v>"qr-payment-order-success" : "QR payment successfully ordered!",</v>
+        <v>"qr-payment" : "QR Payment",</v>
       </c>
       <c r="G43" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A43,""" : """,C43,""",")</f>
-        <v>"qr-payment-order-success" : "QR-Zahlung erfolgreich bestellt!",</v>
+        <v>"qr-payment" : "QR-Zahlung",</v>
       </c>
       <c r="H43" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A43,""" : """,D43,""",")</f>
-        <v>"qr-payment-order-success" : "Pagemento QR è stato ordinato con successo.",</v>
+        <v>"qr-payment" : "Pagamento QR",</v>
       </c>
       <c r="I43" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A43,""" : """,E43,""",")</f>
-        <v>"qr-payment-order-success" : "Le paiement QR a été commandé avec succès!",</v>
+        <v>"qr-payment" : "Paiement QR",</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2550,62 +2670,62 @@
         <v>200</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F44" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A44,""" : """,B44,""",")</f>
-        <v>"quick-tour" : "Quick Tour",</v>
+        <v>"qr-payment-order-success" : "QR payment successfully ordered!",</v>
       </c>
       <c r="G44" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A44,""" : """,C44,""",")</f>
-        <v>"quick-tour" : "Quick Tour",</v>
+        <v>"qr-payment-order-success" : "QR-Zahlung erfolgreich bestellt!",</v>
       </c>
       <c r="H44" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A44,""" : """,D44,""",")</f>
-        <v>"quick-tour" : "Quick Tour (giro)",</v>
+        <v>"qr-payment-order-success" : "Pagemento QR è stato ordinato con successo.",</v>
       </c>
       <c r="I44" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A44,""" : """,E44,""",")</f>
-        <v>"quick-tour" : "Quick Tour",</v>
+        <v>"qr-payment-order-success" : "Le paiement QR a été commandé avec succès!",</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="F45" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A45,""" : """,B45,""",")</f>
-        <v>"region-settings" : "Region Settings",</v>
+        <v>"quick-tour" : "Quick Tour",</v>
       </c>
       <c r="G45" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A45,""" : """,C45,""",")</f>
-        <v>"region-settings" : "Regionenfreischaltung",</v>
+        <v>"quick-tour" : "Quick Tour",</v>
       </c>
       <c r="H45" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A45,""" : """,D45,""",")</f>
-        <v>"region-settings" : "Selezione di regioni",</v>
+        <v>"quick-tour" : "Quick Tour (giro)",</v>
       </c>
       <c r="I45" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A45,""" : """,E45,""",")</f>
-        <v>"region-settings" : "Sélection de régions",</v>
+        <v>"quick-tour" : "Quick Tour",</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2626,19 +2746,19 @@
       </c>
       <c r="F46" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A46,""" : """,B46,""",")</f>
-        <v>"request-new-pin" : "Request New PIN",</v>
+        <v>"region-settings" : "Region Settings",</v>
       </c>
       <c r="G46" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A46,""" : """,C46,""",")</f>
-        <v>"request-new-pin" : "Neuen PIN beantragen",</v>
+        <v>"region-settings" : "Regionenfreischaltung",</v>
       </c>
       <c r="H46" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A46,""" : """,D46,""",")</f>
-        <v>"request-new-pin" : "Richiedere un nuovo PIN",</v>
+        <v>"region-settings" : "Selezione di regioni",</v>
       </c>
       <c r="I46" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A46,""" : """,E46,""",")</f>
-        <v>"request-new-pin" : "Demander nouveau PIN",</v>
+        <v>"region-settings" : "Sélection de régions",</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2659,22 +2779,22 @@
       </c>
       <c r="F47" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A47,""" : """,B47,""",")</f>
-        <v>"reset" : "Reset",</v>
+        <v>"request-new-pin" : "Request New PIN",</v>
       </c>
       <c r="G47" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A47,""" : """,C47,""",")</f>
-        <v>"reset" : "Zurücksetzen",</v>
+        <v>"request-new-pin" : "Neuen PIN beantragen",</v>
       </c>
       <c r="H47" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A47,""" : """,D47,""",")</f>
-        <v>"reset" : "Resettare",</v>
+        <v>"request-new-pin" : "Richiedere un nuovo PIN",</v>
       </c>
       <c r="I47" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A47,""" : """,E47,""",")</f>
-        <v>"reset" : "Réinitialiser",</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"request-new-pin" : "Demander nouveau PIN",</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>217</v>
       </c>
@@ -2692,22 +2812,22 @@
       </c>
       <c r="F48" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A48,""" : """,B48,""",")</f>
-        <v>"run-the-tour-" : "Run the Quick-Tour at any time later by selecting it from the menu.",</v>
+        <v>"reset" : "Reset",</v>
       </c>
       <c r="G48" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A48,""" : """,C48,""",")</f>
-        <v>"run-the-tour-" : "Sie können die Quick-Tour jederzeit später ausführen, indem Sie sie im Menü auswählen.",</v>
+        <v>"reset" : "Zurücksetzen",</v>
       </c>
       <c r="H48" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A48,""" : """,D48,""",")</f>
-        <v>"run-the-tour-" : "Si può sempre prendere il Quick-Tour più tardi, scegliandolo dal menu.",</v>
+        <v>"reset" : "Resettare",</v>
       </c>
       <c r="I48" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A48,""" : """,E48,""",")</f>
-        <v>"run-the-tour-" : "Vour pouvez exécuter le Quick-Tour plus tard si vous le choisissez du menu.",</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"reset" : "Réinitialiser",</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>222</v>
       </c>
@@ -2725,19 +2845,19 @@
       </c>
       <c r="F49" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A49,""" : """,B49,""",")</f>
-        <v>"save" : "Save",</v>
+        <v>"run-the-tour-" : "Run the Quick-Tour at any time later by selecting it from the menu.",</v>
       </c>
       <c r="G49" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A49,""" : """,C49,""",")</f>
-        <v>"save" : "Speichern",</v>
+        <v>"run-the-tour-" : "Sie können die Quick-Tour jederzeit später ausführen, indem Sie sie im Menü auswählen.",</v>
       </c>
       <c r="H49" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A49,""" : """,D49,""",")</f>
-        <v>"save" : "Salvare",</v>
+        <v>"run-the-tour-" : "Si può sempre prendere il Quick-Tour più tardi, scegliandolo dal menu.",</v>
       </c>
       <c r="I49" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A49,""" : """,E49,""",")</f>
-        <v>"save" : "Sauvegarder",</v>
+        <v>"run-the-tour-" : "Vour pouvez exécuter le Quick-Tour plus tard si vous le choisissez du menu.",</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2758,19 +2878,19 @@
       </c>
       <c r="F50" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A50,""" : """,B50,""",")</f>
-        <v>"select-lang" : "Select Language",</v>
+        <v>"save" : "Save",</v>
       </c>
       <c r="G50" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A50,""" : """,C50,""",")</f>
-        <v>"select-lang" : "Sprache wählen",</v>
+        <v>"save" : "Speichern",</v>
       </c>
       <c r="H50" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A50,""" : """,D50,""",")</f>
-        <v>"select-lang" : "Scegli la lingua",</v>
+        <v>"save" : "Salvare",</v>
       </c>
       <c r="I50" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A50,""" : """,E50,""",")</f>
-        <v>"select-lang" : "Choisissez la langue",</v>
+        <v>"save" : "Sauvegarder",</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2791,19 +2911,19 @@
       </c>
       <c r="F51" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A51,""" : """,B51,""",")</f>
-        <v>"send" : "Send",</v>
+        <v>"select-lang" : "Select Language",</v>
       </c>
       <c r="G51" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A51,""" : """,C51,""",")</f>
-        <v>"send" : "Abschicken",</v>
+        <v>"select-lang" : "Sprache wählen",</v>
       </c>
       <c r="H51" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A51,""" : """,D51,""",")</f>
-        <v>"send" : "Spedire",</v>
+        <v>"select-lang" : "Scegli la lingua",</v>
       </c>
       <c r="I51" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A51,""" : """,E51,""",")</f>
-        <v>"send" : "Envoyer",</v>
+        <v>"select-lang" : "Choisissez la langue",</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2824,19 +2944,19 @@
       </c>
       <c r="F52" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A52,""" : """,B52,""",")</f>
-        <v>"settings" : "Settings",</v>
+        <v>"send" : "Send",</v>
       </c>
       <c r="G52" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A52,""" : """,C52,""",")</f>
-        <v>"settings" : "Einstellungen",</v>
+        <v>"send" : "Abschicken",</v>
       </c>
       <c r="H52" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A52,""" : """,D52,""",")</f>
-        <v>"settings" : "Regolazione",</v>
+        <v>"send" : "Spedire",</v>
       </c>
       <c r="I52" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A52,""" : """,E52,""",")</f>
-        <v>"settings" : "Paramètres",</v>
+        <v>"send" : "Envoyer",</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2857,19 +2977,19 @@
       </c>
       <c r="F53" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A53,""" : """,B53,""",")</f>
-        <v>"settings-stored-success" : "Settings successfully stored!",</v>
+        <v>"settings" : "Settings",</v>
       </c>
       <c r="G53" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A53,""" : """,C53,""",")</f>
-        <v>"settings-stored-success" : "Die Einstellungen wurden erfolgreich gespeichert!",</v>
+        <v>"settings" : "Einstellungen",</v>
       </c>
       <c r="H53" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A53,""" : """,D53,""",")</f>
-        <v>"settings-stored-success" : "La regulazione è stata salvata di successo!",</v>
+        <v>"settings" : "Regolazione",</v>
       </c>
       <c r="I53" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A53,""" : """,E53,""",")</f>
-        <v>"settings-stored-success" : "Les paramètres ont étés sauvegardés aves succès!",</v>
+        <v>"settings" : "Paramètres",</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2890,22 +3010,22 @@
       </c>
       <c r="F54" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A54,""" : """,B54,""",")</f>
-        <v>"success" : "Success",</v>
+        <v>"settings-stored-success" : "Settings successfully stored!",</v>
       </c>
       <c r="G54" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A54,""" : """,C54,""",")</f>
-        <v>"success" : "Erfolg",</v>
+        <v>"settings-stored-success" : "Die Einstellungen wurden erfolgreich gespeichert!",</v>
       </c>
       <c r="H54" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A54,""" : """,D54,""",")</f>
-        <v>"success" : "Successo",</v>
+        <v>"settings-stored-success" : "La regulazione è stata salvata di successo!",</v>
       </c>
       <c r="I54" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A54,""" : """,E54,""",")</f>
-        <v>"success" : "Succès",</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"settings-stored-success" : "Les paramètres ont étés sauvegardés aves succès!",</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>252</v>
       </c>
@@ -2923,19 +3043,19 @@
       </c>
       <c r="F55" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A55,""" : """,B55,""",")</f>
-        <v>"swipe-through-the-tour-" : "Swipe through the Quick-Tour to get an overview of MX-Banklets' features.",</v>
+        <v>"success" : "Success",</v>
       </c>
       <c r="G55" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A55,""" : """,C55,""",")</f>
-        <v>"swipe-through-the-tour-" : "Wischen Sie durch die Quick-Tour, um einen Überblick über die Features der MX-Banklets zu bekommen. ",</v>
+        <v>"success" : "Erfolg",</v>
       </c>
       <c r="H55" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A55,""" : """,D55,""",")</f>
-        <v>"swipe-through-the-tour-" : "Passa a traverso il Quick-Tour per ottenere uno sguardo d'insieme delle funzioni die MX-Banklets.",</v>
+        <v>"success" : "Successo",</v>
       </c>
       <c r="I55" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A55,""" : """,E55,""",")</f>
-        <v>"swipe-through-the-tour-" : "Passez par le Quick-Tour pour ramasser une vue d'ensemble des fonctions des MX-Banklets.",</v>
+        <v>"success" : "Succès",</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2956,22 +3076,22 @@
       </c>
       <c r="F56" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A56,""" : """,B56,""",")</f>
-        <v>"take-the-tour-" : "Take the Quick-Tour to get an overview of MX-Banklets' features.",</v>
+        <v>"swipe-through-the-tour-" : "Swipe through the Quick-Tour to get an overview of MX-Banklets' features.",</v>
       </c>
       <c r="G56" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A56,""" : """,C56,""",")</f>
-        <v>"take-the-tour-" : "Nehmen Sie die Quick-Tour, um einen ersten Überblick über die Features von MX-Banklets zu erhalten.",</v>
+        <v>"swipe-through-the-tour-" : "Wischen Sie durch die Quick-Tour, um einen Überblick über die Features der MX-Banklets zu bekommen. ",</v>
       </c>
       <c r="H56" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A56,""" : """,D56,""",")</f>
-        <v>"take-the-tour-" : "Prenda il Quick-Tour per ottenere un primo sguardo sulle funzioni die MX-Banklets.",</v>
+        <v>"swipe-through-the-tour-" : "Passa a traverso il Quick-Tour per ottenere uno sguardo d'insieme delle funzioni die MX-Banklets.",</v>
       </c>
       <c r="I56" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A56,""" : """,E56,""",")</f>
-        <v>"take-the-tour-" : "Prenez le Quick-Tour pour ramasser une vue d'ensemble des fonctions des MX-Banklets.",</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"swipe-through-the-tour-" : "Passez par le Quick-Tour pour ramasser une vue d'ensemble des fonctions des MX-Banklets.",</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>262</v>
       </c>
@@ -2979,67 +3099,67 @@
         <v>263</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F57" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A57,""" : """,B57,""",")</f>
-        <v>"text" : "Text",</v>
+        <v>"take-the-tour-" : "Take the Quick-Tour to get an overview of MX-Banklets' features.",</v>
       </c>
       <c r="G57" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A57,""" : """,C57,""",")</f>
-        <v>"text" : "Text",</v>
+        <v>"take-the-tour-" : "Nehmen Sie die Quick-Tour, um einen ersten Überblick über die Features von MX-Banklets zu erhalten.",</v>
       </c>
       <c r="H57" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A57,""" : """,D57,""",")</f>
-        <v>"text" : "Denominazione",</v>
+        <v>"take-the-tour-" : "Prenda il Quick-Tour per ottenere un primo sguardo sulle funzioni die MX-Banklets.",</v>
       </c>
       <c r="I57" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A57,""" : """,E57,""",")</f>
-        <v>"text" : "Texte",</v>
+        <v>"take-the-tour-" : "Prenez le Quick-Tour pour ramasser une vue d'ensemble des fonctions des MX-Banklets.",</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F58" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A58,""" : """,B58,""",")</f>
-        <v>"to" : "to",</v>
+        <v>"text" : "Text",</v>
       </c>
       <c r="G58" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A58,""" : """,C58,""",")</f>
-        <v>"to" : "bis",</v>
+        <v>"text" : "Text",</v>
       </c>
       <c r="H58" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A58,""" : """,D58,""",")</f>
-        <v>"to" : "Al",</v>
+        <v>"text" : "Denominazione",</v>
       </c>
       <c r="I58" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A58,""" : """,E58,""",")</f>
-        <v>"to" : "au",</v>
+        <v>"text" : "Texte",</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>271</v>
@@ -3051,56 +3171,56 @@
         <v>273</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="F59" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A59,""" : """,B59,""",")</f>
-        <v>"type" : "Type",</v>
+        <v>"to" : "to",</v>
       </c>
       <c r="G59" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A59,""" : """,C59,""",")</f>
-        <v>"type" : "Typ",</v>
+        <v>"to" : "bis",</v>
       </c>
       <c r="H59" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A59,""" : """,D59,""",")</f>
-        <v>"type" : "Tipo",</v>
+        <v>"to" : "Al",</v>
       </c>
       <c r="I59" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A59,""" : """,E59,""",")</f>
-        <v>"type" : "Type",</v>
+        <v>"to" : "au",</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="F60" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A60,""" : """,B60,""",")</f>
-        <v>"unlock-card" : "Unlock Card",</v>
+        <v>"type" : "Type",</v>
       </c>
       <c r="G60" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A60,""" : """,C60,""",")</f>
-        <v>"unlock-card" : "Sperrung aufheben",</v>
+        <v>"type" : "Typ",</v>
       </c>
       <c r="H60" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A60,""" : """,D60,""",")</f>
-        <v>"unlock-card" : "Sbloccare la carta",</v>
+        <v>"type" : "Tipo",</v>
       </c>
       <c r="I60" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A60,""" : """,E60,""",")</f>
-        <v>"unlock-card" : "Débloquer la carte",</v>
+        <v>"type" : "Type",</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3116,27 +3236,27 @@
       <c r="D61" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E61" s="0" t="s">
+      <c r="E61" s="1" t="s">
         <v>283</v>
       </c>
       <c r="F61" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A61,""" : """,B61,""",")</f>
-        <v>"valid-from" : "Valid From",</v>
+        <v>"unlock-card" : "Unlock Card",</v>
       </c>
       <c r="G61" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A61,""" : """,C61,""",")</f>
-        <v>"valid-from" : "Gültig von",</v>
+        <v>"unlock-card" : "Sperrung aufheben",</v>
       </c>
       <c r="H61" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A61,""" : """,D61,""",")</f>
-        <v>"valid-from" : "Valido dal",</v>
+        <v>"unlock-card" : "Sbloccare la carta",</v>
       </c>
       <c r="I61" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A61,""" : """,E61,""",")</f>
-        <v>"valid-from" : "Valable du",</v>
-      </c>
-    </row>
-    <row r="62" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"unlock-card" : "Débloquer la carte",</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>284</v>
       </c>
@@ -3144,62 +3264,62 @@
         <v>285</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>288</v>
       </c>
       <c r="F62" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A62,""" : """,B62,""",")</f>
-        <v>"version" : "Version",</v>
+        <v>"valid-from" : "Valid From",</v>
       </c>
       <c r="G62" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A62,""" : """,C62,""",")</f>
-        <v>"version" : "Version",</v>
+        <v>"valid-from" : "Gültig von",</v>
       </c>
       <c r="H62" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A62,""" : """,D62,""",")</f>
-        <v>"version" : "Versione",</v>
+        <v>"valid-from" : "Valido dal",</v>
       </c>
       <c r="I62" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A62,""" : """,E62,""",")</f>
-        <v>"version" : "Version",</v>
+        <v>"valid-from" : "Valable du",</v>
       </c>
     </row>
     <row r="63" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D63" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="F63" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A63,""" : """,B63,""",")</f>
-        <v>"warning" : "Warning",</v>
+        <v>"version" : "Version",</v>
       </c>
       <c r="G63" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A63,""" : """,C63,""",")</f>
-        <v>"warning" : "Achtung",</v>
+        <v>"version" : "Version",</v>
       </c>
       <c r="H63" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A63,""" : """,D63,""",")</f>
-        <v>"warning" : "Attenzione",</v>
+        <v>"version" : "Versione",</v>
       </c>
       <c r="I63" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A63,""" : """,E63,""",")</f>
-        <v>"warning" : "Attention",</v>
+        <v>"version" : "Version",</v>
       </c>
     </row>
     <row r="64" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3216,110 +3336,238 @@
         <v>295</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F64" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A64,""" : """,B64,""",")</f>
-        <v>"show-confirmations" : "Confirmations",</v>
+        <v>"warning" : "Warning",</v>
       </c>
       <c r="G64" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A64,""" : """,C64,""",")</f>
-        <v>"show-confirmations" : "Bestätigungsmeldungen",</v>
+        <v>"warning" : "Achtung",</v>
       </c>
       <c r="H64" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A64,""" : """,D64,""",")</f>
-        <v>"show-confirmations" : "Confirmazioni",</v>
+        <v>"warning" : "Attenzione",</v>
       </c>
       <c r="I64" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A64,""" : """,E64,""",")</f>
-        <v>"show-confirmations" : "Confirmations",</v>
+        <v>"warning" : "Attention",</v>
       </c>
     </row>
     <row r="65" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>297</v>
       </c>
       <c r="F65" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A65,""" : """,B65,""",")</f>
-        <v>"show-notifications" : "Notifications",</v>
+        <v>"show-confirmations" : "Confirmations",</v>
       </c>
       <c r="G65" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A65,""" : """,C65,""",")</f>
-        <v>"show-notifications" : "Notifizierungen",</v>
+        <v>"show-confirmations" : "Bestätigungsmeldungen",</v>
       </c>
       <c r="H65" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A65,""" : """,D65,""",")</f>
-        <v>"show-notifications" : "Notificazioni",</v>
+        <v>"show-confirmations" : "Confirmazioni",</v>
       </c>
       <c r="I65" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A65,""" : """,E65,""",")</f>
-        <v>"show-notifications" : "Notifications",</v>
+        <v>"show-confirmations" : "Confirmations",</v>
       </c>
     </row>
     <row r="66" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="F66" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A66,""" : """,B66,""",")</f>
-        <v>"yes" : "Yes",</v>
+        <v>"show-notifications" : "Notifications",</v>
       </c>
       <c r="G66" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A66,""" : """,C66,""",")</f>
-        <v>"yes" : "Ja",</v>
+        <v>"show-notifications" : "Notifizierungen",</v>
       </c>
       <c r="H66" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A66,""" : """,D66,""",")</f>
-        <v>"yes" : "Sì",</v>
+        <v>"show-notifications" : "Notificazioni",</v>
       </c>
       <c r="I66" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A66,""" : """,E66,""",")</f>
+        <v>"show-notifications" : "Notifications",</v>
+      </c>
+    </row>
+    <row r="67" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="F67" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A67,""" : """,B67,""",")</f>
+        <v>"enter-username-pwd" : "Please enter username 'test' and password 'test'!",</v>
+      </c>
+      <c r="G67" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A67,""" : """,C67,""",")</f>
+        <v>"enter-username-pwd" : "Bitte Benutzername 'test' und Passwort 'test' eingeben!",</v>
+      </c>
+      <c r="H67" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A67,""" : """,D67,""",")</f>
+        <v>"enter-username-pwd" : "Pregasi immetere il nome dell utente 'test' e la parola d‘accesso 'test'!",</v>
+      </c>
+      <c r="I67" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A67,""" : """,E67,""",")</f>
+        <v>"enter-username-pwd" : "Entrez le nom d‘utilisateur 'test' et le mot de passe 'test', s.v.p.!",</v>
+      </c>
+    </row>
+    <row r="68" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F68" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A68,""" : """,B68,""",")</f>
+        <v>"start-the-tour" : "Start the tour…",</v>
+      </c>
+      <c r="G68" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A68,""" : """,C68,""",")</f>
+        <v>"start-the-tour" : "Beginne die Tour…",</v>
+      </c>
+      <c r="H68" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A68,""" : """,D68,""",")</f>
+        <v>"start-the-tour" : "Incomincia il giro…",</v>
+      </c>
+      <c r="I68" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A68,""" : """,E68,""",")</f>
+        <v>"start-the-tour" : "Commencez le tour…",</v>
+      </c>
+    </row>
+    <row r="69" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F69" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A69,""" : """,B69,""",")</f>
+        <v>"username" : "Username",</v>
+      </c>
+      <c r="G69" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A69,""" : """,C69,""",")</f>
+        <v>"username" : "Benutzername",</v>
+      </c>
+      <c r="H69" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A69,""" : """,D69,""",")</f>
+        <v>"username" : "Nome utente",</v>
+      </c>
+      <c r="I69" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A69,""" : """,E69,""",")</f>
+        <v>"username" : "Nom d'utilisateur",</v>
+      </c>
+    </row>
+    <row r="70" s="3" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F70" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A70,""" : """,B70,""",")</f>
+        <v>"yes" : "Yes",</v>
+      </c>
+      <c r="G70" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A70,""" : """,C70,""",")</f>
+        <v>"yes" : "Ja",</v>
+      </c>
+      <c r="H70" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A70,""" : """,D70,""",")</f>
+        <v>"yes" : "Sì",</v>
+      </c>
+      <c r="I70" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A70,""" : """,E70,""",")</f>
         <v>"yes" : "Oui",</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F67" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="68" s="4" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F71" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="72" s="4" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
fix nav menu translations and swipe direction of quck tour
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="336">
   <si>
     <t xml:space="preserve">KEY</t>
   </si>
@@ -379,6 +379,21 @@
     <t xml:space="preserve">Travailler</t>
   </si>
   <si>
+    <t xml:space="preserve">enter-username-pwd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter username 'test' and password 'test'!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bitte Benutzername 'test' und Passwort 'test' eingeben!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pregasi immetere il nome dell utente 'test' e la parola d‘accesso 'test'!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrez le nom d‘utilisateur 'test' et le mot de passe 'test', s.v.p.!</t>
+  </si>
+  <si>
     <t xml:space="preserve">error</t>
   </si>
   <si>
@@ -394,6 +409,15 @@
     <t xml:space="preserve">Erreur</t>
   </si>
   <si>
+    <t xml:space="preserve">info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informazione</t>
+  </si>
+  <si>
     <t xml:space="preserve">liechtenstein</t>
   </si>
   <si>
@@ -439,6 +463,12 @@
     <t xml:space="preserve">Bloquer / Débloquer</t>
   </si>
   <si>
+    <t xml:space="preserve">login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login</t>
+  </si>
+  <si>
     <t xml:space="preserve">logout</t>
   </si>
   <si>
@@ -574,6 +604,21 @@
     <t xml:space="preserve">Commander</t>
   </si>
   <si>
+    <t xml:space="preserve">order-qr-payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To order a QR payment, please provide account and amount!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Konto und Betrag müssen ausgefüllt sein, damit eine QR-Zahlung bestellt werden kann!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si prega di mettere a disposizione il conto e il montante per potere ordinare il pagamento QR! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compte et montant doivent être remplis avant de commander un paiement QR!</t>
+  </si>
+  <si>
     <t xml:space="preserve">password</t>
   </si>
   <si>
@@ -589,21 +634,6 @@
     <t xml:space="preserve">Mot de passe</t>
   </si>
   <si>
-    <t xml:space="preserve">order-qr-payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To order a QR payment, please provide account and amount!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Konto und Betrag müssen ausgefüllt sein, damit eine QR-Zahlung bestellt werden kann!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si prega di mettere a disposizione il conto e il montante per potere ordinare il pagamento QR! </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compte et montant doivent être remplis avant de commander un paiement QR!</t>
-  </si>
-  <si>
     <t xml:space="preserve">qr-payment</t>
   </si>
   <si>
@@ -628,46 +658,10 @@
     <t xml:space="preserve">QR-Bargeldbezug erfolgreich bestellt!</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Riferimento contante</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> QR è stato ordinato con successo.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Retrait de liquide </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">QR a été commandé avec succès!</t>
-    </r>
+    <t xml:space="preserve">Riferimento contante QR è stato ordinato con successo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retrait de liquide QR a été commandé avec succès!</t>
   </si>
   <si>
     <t xml:space="preserve">quick-tour</t>
@@ -694,6 +688,21 @@
     <t xml:space="preserve">Sélection de régions</t>
   </si>
   <si>
+    <t xml:space="preserve">register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registrieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registrare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enregistrer</t>
+  </si>
+  <si>
     <t xml:space="preserve">request-new-pin</t>
   </si>
   <si>
@@ -814,6 +823,45 @@
     <t xml:space="preserve">Les paramètres ont étés sauvegardés aves succès!</t>
   </si>
   <si>
+    <t xml:space="preserve">show-confirmations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirmations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bestätigungsmeldungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirmazioni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show-notifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notifizierungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notificazioni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start-the-tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start the tour…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beginne die Tour…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incomincia il giro…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commencez le tour…</t>
+  </si>
+  <si>
     <t xml:space="preserve">success</t>
   </si>
   <si>
@@ -910,6 +958,21 @@
     <t xml:space="preserve">Débloquer la carte</t>
   </si>
   <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benutzername</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome utente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom d'utilisateur</t>
+  </si>
+  <si>
     <t xml:space="preserve">valid-from</t>
   </si>
   <si>
@@ -947,129 +1010,6 @@
   </si>
   <si>
     <t xml:space="preserve">Attention</t>
-  </si>
-  <si>
-    <t xml:space="preserve">show-confirmations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Confirmations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bestätigungsmeldungen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Confirmazioni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">show-notifications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notifications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notifizierungen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notificazioni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enter-username-pwd</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Please enter username </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'test' and password 'test'!</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Bitte Benutzername 'test' und Passwort 'test' eingeben!</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Pregasi immetere il nome dell utente </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'test' e la parola d‘accesso 'test'!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Entrez le nom d‘utilisateur </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'test' et le mot de passe 'test', s.v.p.!</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">start-the-tour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start the tour…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beginne die Tour…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incomincia il giro…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commencez le tour…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benutzername</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nome utente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom d'utilisateur</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -1097,7 +1037,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1128,12 +1068,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1197,11 +1131,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1288,8 +1222,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2:I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
@@ -2088,24 +2022,24 @@
       <c r="D25" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="3" t="s">
         <v>123</v>
       </c>
       <c r="F25" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A25,""" : """,B25,""",")</f>
-        <v>"error" : "Error",</v>
+        <v>"enter-username-pwd" : "Please enter username 'test' and password 'test'!",</v>
       </c>
       <c r="G25" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A25,""" : """,C25,""",")</f>
-        <v>"error" : "Fehler",</v>
+        <v>"enter-username-pwd" : "Bitte Benutzername 'test' und Passwort 'test' eingeben!",</v>
       </c>
       <c r="H25" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A25,""" : """,D25,""",")</f>
-        <v>"error" : "Errore",</v>
+        <v>"enter-username-pwd" : "Pregasi immetere il nome dell utente 'test' e la parola d‘accesso 'test'!",</v>
       </c>
       <c r="I25" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A25,""" : """,E25,""",")</f>
-        <v>"error" : "Erreur",</v>
+        <v>"enter-username-pwd" : "Entrez le nom d‘utilisateur 'test' et le mot de passe 'test', s.v.p.!",</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,95 +2050,95 @@
         <v>125</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F26" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A26,""" : """,B26,""",")</f>
-        <v>"liechtenstein" : "Liechtenstein",</v>
+        <v>"error" : "Error",</v>
       </c>
       <c r="G26" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A26,""" : """,C26,""",")</f>
-        <v>"liechtenstein" : "Liechtenstein",</v>
+        <v>"error" : "Fehler",</v>
       </c>
       <c r="H26" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A26,""" : """,D26,""",")</f>
-        <v>"liechtenstein" : "Liechtenstein",</v>
+        <v>"error" : "Errore",</v>
       </c>
       <c r="I26" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A26,""" : """,E26,""",")</f>
-        <v>"liechtenstein" : "Liechtenstein",</v>
+        <v>"error" : "Erreur",</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F27" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A27,""" : """,B27,""",")</f>
-        <v>"limit" : "Limit",</v>
+        <v>"info" : "Information",</v>
       </c>
       <c r="G27" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A27,""" : """,C27,""",")</f>
-        <v>"limit" : "Limite",</v>
+        <v>"info" : "Information",</v>
       </c>
       <c r="H27" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A27,""" : """,D27,""",")</f>
-        <v>"limit" : "Limite",</v>
+        <v>"info" : "Informazione",</v>
       </c>
       <c r="I27" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A27,""" : """,E27,""",")</f>
-        <v>"limit" : "Limite",</v>
+        <v>"info" : "Information",</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>133</v>
       </c>
       <c r="F28" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A28,""" : """,B28,""",")</f>
-        <v>"lock-card" : "Lock Card",</v>
+        <v>"liechtenstein" : "Liechtenstein",</v>
       </c>
       <c r="G28" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A28,""" : """,C28,""",")</f>
-        <v>"lock-card" : "Karte sperren",</v>
+        <v>"liechtenstein" : "Liechtenstein",</v>
       </c>
       <c r="H28" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A28,""" : """,D28,""",")</f>
-        <v>"lock-card" : "Bloccare la carta",</v>
+        <v>"liechtenstein" : "Liechtenstein",</v>
       </c>
       <c r="I28" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A28,""" : """,E28,""",")</f>
-        <v>"lock-card" : "Bloquer la carte",</v>
+        <v>"liechtenstein" : "Liechtenstein",</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,1330 +2152,1330 @@
         <v>136</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F29" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A29,""" : """,B29,""",")</f>
-        <v>"lock-unlock" : "Lock / Unlock",</v>
+        <v>"limit" : "Limit",</v>
       </c>
       <c r="G29" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A29,""" : """,C29,""",")</f>
-        <v>"lock-unlock" : "Sperren / Entsperren",</v>
+        <v>"limit" : "Limite",</v>
       </c>
       <c r="H29" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A29,""" : """,D29,""",")</f>
-        <v>"lock-unlock" : "Bloccare / Sbloccare",</v>
+        <v>"limit" : "Limite",</v>
       </c>
       <c r="I29" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A29,""" : """,E29,""",")</f>
-        <v>"lock-unlock" : "Bloquer / Débloquer",</v>
+        <v>"limit" : "Limite",</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>140</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F30" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A30,""" : """,B30,""",")</f>
-        <v>"logout" : "Logout",</v>
+        <v>"lock-card" : "Lock Card",</v>
       </c>
       <c r="G30" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A30,""" : """,C30,""",")</f>
-        <v>"logout" : "Logout",</v>
+        <v>"lock-card" : "Karte sperren",</v>
       </c>
       <c r="H30" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A30,""" : """,D30,""",")</f>
-        <v>"logout" : "Logout",</v>
+        <v>"lock-card" : "Bloccare la carta",</v>
       </c>
       <c r="I30" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A30,""" : """,E30,""",")</f>
-        <v>"logout" : "Logout",</v>
+        <v>"lock-card" : "Bloquer la carte",</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D31" s="0" t="s">
         <v>144</v>
       </c>
+      <c r="D31" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E31" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F31" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A31,""" : """,B31,""",")</f>
-        <v>"mask-reset-success" : "Input mask successfully reset!",</v>
+        <v>"lock-unlock" : "Lock / Unlock",</v>
       </c>
       <c r="G31" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A31,""" : """,C31,""",")</f>
-        <v>"mask-reset-success" : "Eingabemaske erfolgreich zurückgesetzt!",</v>
+        <v>"lock-unlock" : "Sperren / Entsperren",</v>
       </c>
       <c r="H31" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A31,""" : """,D31,""",")</f>
-        <v>"mask-reset-success" : "Campi di input resettati con successo!",</v>
+        <v>"lock-unlock" : "Bloccare / Sbloccare",</v>
       </c>
       <c r="I31" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A31,""" : """,E31,""",")</f>
-        <v>"mask-reset-success" : "Cadres réinitilisés avec succès!",</v>
+        <v>"lock-unlock" : "Bloquer / Débloquer",</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>148</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F32" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A32,""" : """,B32,""",")</f>
-        <v>"monthly-limit" : "Monthly Limit",</v>
+        <v>"login" : "Login",</v>
       </c>
       <c r="G32" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A32,""" : """,C32,""",")</f>
-        <v>"monthly-limit" : "Monatslimite",</v>
+        <v>"login" : "Login",</v>
       </c>
       <c r="H32" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A32,""" : """,D32,""",")</f>
-        <v>"monthly-limit" : "Limite mensile",</v>
+        <v>"login" : "Login",</v>
       </c>
       <c r="I32" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A32,""" : """,E32,""",")</f>
-        <v>"monthly-limit" : "Limite mensuelle",</v>
+        <v>"login" : "Login",</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F33" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A33,""" : """,B33,""",")</f>
-        <v>"mx-banklets" : "MX-Banklets",</v>
+        <v>"logout" : "Logout",</v>
       </c>
       <c r="G33" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A33,""" : """,C33,""",")</f>
-        <v>"mx-banklets" : "MX-Banklets",</v>
+        <v>"logout" : "Logout",</v>
       </c>
       <c r="H33" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A33,""" : """,D33,""",")</f>
-        <v>"mx-banklets" : "MX-Banklets",</v>
+        <v>"logout" : "Logout",</v>
       </c>
       <c r="I33" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A33,""" : """,E33,""",")</f>
-        <v>"mx-banklets" : "MX-Banklets",</v>
+        <v>"logout" : "Logout",</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="D34" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="F34" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A34,""" : """,B34,""",")</f>
-        <v>"new-pin" : "New PIN",</v>
+        <v>"mask-reset-success" : "Input mask successfully reset!",</v>
       </c>
       <c r="G34" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A34,""" : """,C34,""",")</f>
-        <v>"new-pin" : "Neuer PIN",</v>
+        <v>"mask-reset-success" : "Eingabemaske erfolgreich zurückgesetzt!",</v>
       </c>
       <c r="H34" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A34,""" : """,D34,""",")</f>
-        <v>"new-pin" : "Nuovo PIN",</v>
+        <v>"mask-reset-success" : "Campi di input resettati con successo!",</v>
       </c>
       <c r="I34" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A34,""" : """,E34,""",")</f>
-        <v>"new-pin" : "Nouveau PIN",</v>
+        <v>"mask-reset-success" : "Cadres réinitilisés avec succès!",</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="F35" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A35,""" : """,B35,""",")</f>
-        <v>"new-pin-request-success" : "New PIN successfully requested!",</v>
+        <v>"monthly-limit" : "Monthly Limit",</v>
       </c>
       <c r="G35" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A35,""" : """,C35,""",")</f>
-        <v>"new-pin-request-success" : "Neuer PIN erfolgreich beantragt!",</v>
+        <v>"monthly-limit" : "Monatslimite",</v>
       </c>
       <c r="H35" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A35,""" : """,D35,""",")</f>
-        <v>"new-pin-request-success" : "Nuovo PIN richiesto con successo!",</v>
+        <v>"monthly-limit" : "Limite mensile",</v>
       </c>
       <c r="I35" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A35,""" : """,E35,""",")</f>
-        <v>"new-pin-request-success" : "Un nouveau PIN a été demandé avec succès!",</v>
+        <v>"monthly-limit" : "Limite mensuelle",</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F36" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A36,""" : """,B36,""",")</f>
-        <v>"no" : "No",</v>
+        <v>"mx-banklets" : "MX-Banklets",</v>
       </c>
       <c r="G36" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A36,""" : """,C36,""",")</f>
-        <v>"no" : "Nein",</v>
+        <v>"mx-banklets" : "MX-Banklets",</v>
       </c>
       <c r="H36" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A36,""" : """,D36,""",")</f>
-        <v>"no" : "No",</v>
+        <v>"mx-banklets" : "MX-Banklets",</v>
       </c>
       <c r="I36" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A36,""" : """,E36,""",")</f>
-        <v>"no" : "Non",</v>
+        <v>"mx-banklets" : "MX-Banklets",</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="F37" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A37,""" : """,B37,""",")</f>
-        <v>"no-changes-no-reset" : "No changes, nothing to undo.",</v>
+        <v>"new-pin" : "New PIN",</v>
       </c>
       <c r="G37" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A37,""" : """,C37,""",")</f>
-        <v>"no-changes-no-reset" : "Keine Änderungen, nichts zurückzusetzen.",</v>
+        <v>"new-pin" : "Neuer PIN",</v>
       </c>
       <c r="H37" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A37,""" : """,D37,""",")</f>
-        <v>"no-changes-no-reset" : "Non ci sono modificazioni, niente da resettare.",</v>
+        <v>"new-pin" : "Nuovo PIN",</v>
       </c>
       <c r="I37" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A37,""" : """,E37,""",")</f>
-        <v>"no-changes-no-reset" : "Il n‘y a pas de modifications à réinitialiser.",</v>
+        <v>"new-pin" : "Nouveau PIN",</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="F38" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A38,""" : """,B38,""",")</f>
-        <v>"no-changes-no-save" : "No changes, nothing to save.",</v>
+        <v>"new-pin-request-success" : "New PIN successfully requested!",</v>
       </c>
       <c r="G38" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A38,""" : """,C38,""",")</f>
-        <v>"no-changes-no-save" : "Keine Änderungen, nichts zu speichern.",</v>
+        <v>"new-pin-request-success" : "Neuer PIN erfolgreich beantragt!",</v>
       </c>
       <c r="H38" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A38,""" : """,D38,""",")</f>
-        <v>"no-changes-no-save" : "Non ci sono modificazioni, niente da salvare.",</v>
+        <v>"new-pin-request-success" : "Nuovo PIN richiesto con successo!",</v>
       </c>
       <c r="I38" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A38,""" : """,E38,""",")</f>
-        <v>"no-changes-no-save" : "Il n‘y a pas de modifications à sauvegarder.",</v>
+        <v>"new-pin-request-success" : "Un nouveau PIN a été demandé avec succès!",</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F39" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A39,""" : """,B39,""",")</f>
-        <v>"ok" : "OK",</v>
+        <v>"no" : "No",</v>
       </c>
       <c r="G39" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A39,""" : """,C39,""",")</f>
-        <v>"ok" : "OK",</v>
+        <v>"no" : "Nein",</v>
       </c>
       <c r="H39" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A39,""" : """,D39,""",")</f>
-        <v>"ok" : "OK",</v>
+        <v>"no" : "No",</v>
       </c>
       <c r="I39" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A39,""" : """,E39,""",")</f>
-        <v>"ok" : "OK",</v>
+        <v>"no" : "Non",</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="F40" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A40,""" : """,B40,""",")</f>
-        <v>"order" : "Order",</v>
+        <v>"no-changes-no-reset" : "No changes, nothing to undo.",</v>
       </c>
       <c r="G40" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A40,""" : """,C40,""",")</f>
-        <v>"order" : "Bestellen",</v>
+        <v>"no-changes-no-reset" : "Keine Änderungen, nichts zurückzusetzen.",</v>
       </c>
       <c r="H40" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A40,""" : """,D40,""",")</f>
-        <v>"order" : "Ordinare",</v>
+        <v>"no-changes-no-reset" : "Non ci sono modificazioni, niente da resettare.",</v>
       </c>
       <c r="I40" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A40,""" : """,E40,""",")</f>
-        <v>"order" : "Commander",</v>
+        <v>"no-changes-no-reset" : "Il n‘y a pas de modifications à réinitialiser.",</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="F41" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A41,""" : """,B41,""",")</f>
-        <v>"password" : "Password",</v>
+        <v>"no-changes-no-save" : "No changes, nothing to save.",</v>
       </c>
       <c r="G41" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A41,""" : """,C41,""",")</f>
-        <v>"password" : "Passwort",</v>
+        <v>"no-changes-no-save" : "Keine Änderungen, nichts zu speichern.",</v>
       </c>
       <c r="H41" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A41,""" : """,D41,""",")</f>
-        <v>"password" : "Parola d'accesso",</v>
+        <v>"no-changes-no-save" : "Non ci sono modificazioni, niente da salvare.",</v>
       </c>
       <c r="I41" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A41,""" : """,E41,""",")</f>
-        <v>"password" : "Mot de passe",</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"no-changes-no-save" : "Il n‘y a pas de modifications à sauvegarder.",</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F42" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A42,""" : """,B42,""",")</f>
-        <v>"order-qr-payment" : "To order a QR payment, please provide account and amount!",</v>
+        <v>"ok" : "OK",</v>
       </c>
       <c r="G42" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A42,""" : """,C42,""",")</f>
-        <v>"order-qr-payment" : "Konto und Betrag müssen ausgefüllt sein, damit eine QR-Zahlung bestellt werden kann!",</v>
+        <v>"ok" : "OK",</v>
       </c>
       <c r="H42" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A42,""" : """,D42,""",")</f>
-        <v>"order-qr-payment" : "Si prega di mettere a disposizione il conto e il montante per potere ordinare il pagamento QR! ",</v>
+        <v>"ok" : "OK",</v>
       </c>
       <c r="I42" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A42,""" : """,E42,""",")</f>
-        <v>"order-qr-payment" : "Compte et montant doivent être remplis avant de commander un paiement QR!",</v>
+        <v>"ok" : "OK",</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F43" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A43,""" : """,B43,""",")</f>
-        <v>"qr-payment" : "QR Cash Withdrawal",</v>
+        <v>"order" : "Order",</v>
       </c>
       <c r="G43" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A43,""" : """,C43,""",")</f>
-        <v>"qr-payment" : "QR-Bargeldbezug",</v>
+        <v>"order" : "Bestellen",</v>
       </c>
       <c r="H43" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A43,""" : """,D43,""",")</f>
-        <v>"qr-payment" : "Riferimento contante QR",</v>
+        <v>"order" : "Ordinare",</v>
       </c>
       <c r="I43" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A43,""" : """,E43,""",")</f>
-        <v>"qr-payment" : "Retrait de liquide QR",</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"order" : "Commander",</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="F44" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A44,""" : """,B44,""",")</f>
-        <v>"qr-payment-order-success" : "QR cash withdrawal successfully ordered!",</v>
+        <v>"order-qr-payment" : "To order a QR payment, please provide account and amount!",</v>
       </c>
       <c r="G44" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A44,""" : """,C44,""",")</f>
-        <v>"qr-payment-order-success" : "QR-Bargeldbezug erfolgreich bestellt!",</v>
+        <v>"order-qr-payment" : "Konto und Betrag müssen ausgefüllt sein, damit eine QR-Zahlung bestellt werden kann!",</v>
       </c>
       <c r="H44" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A44,""" : """,D44,""",")</f>
-        <v>"qr-payment-order-success" : "Riferimento contante QR è stato ordinato con successo.",</v>
+        <v>"order-qr-payment" : "Si prega di mettere a disposizione il conto e il montante per potere ordinare il pagamento QR! ",</v>
       </c>
       <c r="I44" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A44,""" : """,E44,""",")</f>
-        <v>"qr-payment-order-success" : "Retrait de liquide QR a été commandé avec succès!",</v>
+        <v>"order-qr-payment" : "Compte et montant doivent être remplis avant de commander un paiement QR!",</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F45" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A45,""" : """,B45,""",")</f>
-        <v>"quick-tour" : "Quick Tour",</v>
+        <v>"password" : "Password",</v>
       </c>
       <c r="G45" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A45,""" : """,C45,""",")</f>
-        <v>"quick-tour" : "Quick Tour",</v>
+        <v>"password" : "Passwort",</v>
       </c>
       <c r="H45" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A45,""" : """,D45,""",")</f>
-        <v>"quick-tour" : "Quick Tour (giro)",</v>
+        <v>"password" : "Parola d'accesso",</v>
       </c>
       <c r="I45" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A45,""" : """,E45,""",")</f>
-        <v>"quick-tour" : "Quick Tour",</v>
+        <v>"password" : "Mot de passe",</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="F46" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A46,""" : """,B46,""",")</f>
-        <v>"region-settings" : "Region Settings",</v>
+        <v>"qr-payment" : "QR Cash Withdrawal",</v>
       </c>
       <c r="G46" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A46,""" : """,C46,""",")</f>
-        <v>"region-settings" : "Regionenfreischaltung",</v>
+        <v>"qr-payment" : "QR-Bargeldbezug",</v>
       </c>
       <c r="H46" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A46,""" : """,D46,""",")</f>
-        <v>"region-settings" : "Selezione di regioni",</v>
+        <v>"qr-payment" : "Riferimento contante QR",</v>
       </c>
       <c r="I46" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A46,""" : """,E46,""",")</f>
-        <v>"region-settings" : "Sélection de régions",</v>
+        <v>"qr-payment" : "Retrait de liquide QR",</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D47" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="E47" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="F47" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A47,""" : """,B47,""",")</f>
-        <v>"request-new-pin" : "Request New PIN",</v>
+        <v>"qr-payment-order-success" : "QR cash withdrawal successfully ordered!",</v>
       </c>
       <c r="G47" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A47,""" : """,C47,""",")</f>
-        <v>"request-new-pin" : "Neuen PIN beantragen",</v>
+        <v>"qr-payment-order-success" : "QR-Bargeldbezug erfolgreich bestellt!",</v>
       </c>
       <c r="H47" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A47,""" : """,D47,""",")</f>
-        <v>"request-new-pin" : "Richiedere un nuovo PIN",</v>
+        <v>"qr-payment-order-success" : "Riferimento contante QR è stato ordinato con successo.",</v>
       </c>
       <c r="I47" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A47,""" : """,E47,""",")</f>
-        <v>"request-new-pin" : "Demander nouveau PIN",</v>
+        <v>"qr-payment-order-success" : "Retrait de liquide QR a été commandé avec succès!",</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="F48" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A48,""" : """,B48,""",")</f>
-        <v>"reset" : "Reset",</v>
+        <v>"quick-tour" : "Quick Tour",</v>
       </c>
       <c r="G48" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A48,""" : """,C48,""",")</f>
-        <v>"reset" : "Zurücksetzen",</v>
+        <v>"quick-tour" : "Quick Tour",</v>
       </c>
       <c r="H48" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A48,""" : """,D48,""",")</f>
-        <v>"reset" : "Resettare",</v>
+        <v>"quick-tour" : "Quick Tour (giro)",</v>
       </c>
       <c r="I48" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A48,""" : """,E48,""",")</f>
-        <v>"reset" : "Réinitialiser",</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"quick-tour" : "Quick Tour",</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F49" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A49,""" : """,B49,""",")</f>
-        <v>"run-the-tour-" : "Run the Quick-Tour at any time later by selecting it from the menu.",</v>
+        <v>"region-settings" : "Region Settings",</v>
       </c>
       <c r="G49" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A49,""" : """,C49,""",")</f>
-        <v>"run-the-tour-" : "Sie können die Quick-Tour jederzeit später ausführen, indem Sie sie im Menü auswählen.",</v>
+        <v>"region-settings" : "Regionenfreischaltung",</v>
       </c>
       <c r="H49" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A49,""" : """,D49,""",")</f>
-        <v>"run-the-tour-" : "Si può sempre prendere il Quick-Tour più tardi, scegliandolo dal menu.",</v>
+        <v>"region-settings" : "Selezione di regioni",</v>
       </c>
       <c r="I49" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A49,""" : """,E49,""",")</f>
-        <v>"run-the-tour-" : "Vour pouvez exécuter le Quick-Tour plus tard si vous le choisissez du menu.",</v>
+        <v>"region-settings" : "Sélection de régions",</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F50" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A50,""" : """,B50,""",")</f>
-        <v>"save" : "Save",</v>
+        <v>"register" : "Register",</v>
       </c>
       <c r="G50" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A50,""" : """,C50,""",")</f>
-        <v>"save" : "Speichern",</v>
+        <v>"register" : "Registrieren",</v>
       </c>
       <c r="H50" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A50,""" : """,D50,""",")</f>
-        <v>"save" : "Salvare",</v>
+        <v>"register" : "Registrare",</v>
       </c>
       <c r="I50" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A50,""" : """,E50,""",")</f>
-        <v>"save" : "Sauvegarder",</v>
+        <v>"register" : "Enregistrer",</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F51" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A51,""" : """,B51,""",")</f>
-        <v>"select-lang" : "Select Language",</v>
+        <v>"request-new-pin" : "Request New PIN",</v>
       </c>
       <c r="G51" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A51,""" : """,C51,""",")</f>
-        <v>"select-lang" : "Sprache wählen",</v>
+        <v>"request-new-pin" : "Neuen PIN beantragen",</v>
       </c>
       <c r="H51" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A51,""" : """,D51,""",")</f>
-        <v>"select-lang" : "Scegli la lingua",</v>
+        <v>"request-new-pin" : "Richiedere un nuovo PIN",</v>
       </c>
       <c r="I51" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A51,""" : """,E51,""",")</f>
-        <v>"select-lang" : "Choisissez la langue",</v>
+        <v>"request-new-pin" : "Demander nouveau PIN",</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F52" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A52,""" : """,B52,""",")</f>
-        <v>"send" : "Send",</v>
+        <v>"reset" : "Reset",</v>
       </c>
       <c r="G52" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A52,""" : """,C52,""",")</f>
-        <v>"send" : "Abschicken",</v>
+        <v>"reset" : "Zurücksetzen",</v>
       </c>
       <c r="H52" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A52,""" : """,D52,""",")</f>
-        <v>"send" : "Spedire",</v>
+        <v>"reset" : "Resettare",</v>
       </c>
       <c r="I52" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A52,""" : """,E52,""",")</f>
-        <v>"send" : "Envoyer",</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"reset" : "Réinitialiser",</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F53" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A53,""" : """,B53,""",")</f>
-        <v>"settings" : "Settings",</v>
+        <v>"run-the-tour-" : "Run the Quick-Tour at any time later by selecting it from the menu.",</v>
       </c>
       <c r="G53" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A53,""" : """,C53,""",")</f>
-        <v>"settings" : "Einstellungen",</v>
+        <v>"run-the-tour-" : "Sie können die Quick-Tour jederzeit später ausführen, indem Sie sie im Menü auswählen.",</v>
       </c>
       <c r="H53" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A53,""" : """,D53,""",")</f>
-        <v>"settings" : "Regolazione",</v>
+        <v>"run-the-tour-" : "Si può sempre prendere il Quick-Tour più tardi, scegliandolo dal menu.",</v>
       </c>
       <c r="I53" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A53,""" : """,E53,""",")</f>
-        <v>"settings" : "Paramètres",</v>
+        <v>"run-the-tour-" : "Vour pouvez exécuter le Quick-Tour plus tard si vous le choisissez du menu.",</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F54" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A54,""" : """,B54,""",")</f>
-        <v>"settings-stored-success" : "Settings successfully stored!",</v>
+        <v>"save" : "Save",</v>
       </c>
       <c r="G54" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A54,""" : """,C54,""",")</f>
-        <v>"settings-stored-success" : "Die Einstellungen wurden erfolgreich gespeichert!",</v>
+        <v>"save" : "Speichern",</v>
       </c>
       <c r="H54" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A54,""" : """,D54,""",")</f>
-        <v>"settings-stored-success" : "La regulazione è stata salvata di successo!",</v>
+        <v>"save" : "Salvare",</v>
       </c>
       <c r="I54" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A54,""" : """,E54,""",")</f>
-        <v>"settings-stored-success" : "Les paramètres ont étés sauvegardés aves succès!",</v>
+        <v>"save" : "Sauvegarder",</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F55" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A55,""" : """,B55,""",")</f>
-        <v>"success" : "Success",</v>
+        <v>"select-lang" : "Select Language",</v>
       </c>
       <c r="G55" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A55,""" : """,C55,""",")</f>
-        <v>"success" : "Erfolg",</v>
+        <v>"select-lang" : "Sprache wählen",</v>
       </c>
       <c r="H55" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A55,""" : """,D55,""",")</f>
-        <v>"success" : "Successo",</v>
+        <v>"select-lang" : "Scegli la lingua",</v>
       </c>
       <c r="I55" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A55,""" : """,E55,""",")</f>
-        <v>"success" : "Succès",</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"select-lang" : "Choisissez la langue",</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="F56" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A56,""" : """,B56,""",")</f>
-        <v>"swipe-through-the-tour-" : "Swipe through the Quick-Tour to get an overview of MX-Banklets' features.",</v>
+        <v>"send" : "Send",</v>
       </c>
       <c r="G56" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A56,""" : """,C56,""",")</f>
-        <v>"swipe-through-the-tour-" : "Wischen Sie durch die Quick-Tour, um einen Überblick über die Features der MX-Banklets zu bekommen. ",</v>
+        <v>"send" : "Abschicken",</v>
       </c>
       <c r="H56" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A56,""" : """,D56,""",")</f>
-        <v>"swipe-through-the-tour-" : "Passa a traverso il Quick-Tour per ottenere uno sguardo d'insieme delle funzioni die MX-Banklets.",</v>
+        <v>"send" : "Spedire",</v>
       </c>
       <c r="I56" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A56,""" : """,E56,""",")</f>
-        <v>"swipe-through-the-tour-" : "Passez par le Quick-Tour pour ramasser une vue d'ensemble des fonctions des MX-Banklets.",</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"send" : "Envoyer",</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F57" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A57,""" : """,B57,""",")</f>
-        <v>"take-the-tour-" : "Take the Quick-Tour to get an overview of MX-Banklets' features.",</v>
+        <v>"settings" : "Settings",</v>
       </c>
       <c r="G57" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A57,""" : """,C57,""",")</f>
-        <v>"take-the-tour-" : "Nehmen Sie die Quick-Tour, um einen ersten Überblick über die Features von MX-Banklets zu erhalten.",</v>
+        <v>"settings" : "Einstellungen",</v>
       </c>
       <c r="H57" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A57,""" : """,D57,""",")</f>
-        <v>"take-the-tour-" : "Prenda il Quick-Tour per ottenere un primo sguardo sulle funzioni die MX-Banklets.",</v>
+        <v>"settings" : "Regolazione",</v>
       </c>
       <c r="I57" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A57,""" : """,E57,""",")</f>
-        <v>"take-the-tour-" : "Prenez le Quick-Tour pour ramasser une vue d'ensemble des fonctions des MX-Banklets.",</v>
+        <v>"settings" : "Paramètres",</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F58" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A58,""" : """,B58,""",")</f>
-        <v>"text" : "Text",</v>
+        <v>"settings-stored-success" : "Settings successfully stored!",</v>
       </c>
       <c r="G58" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A58,""" : """,C58,""",")</f>
-        <v>"text" : "Text",</v>
+        <v>"settings-stored-success" : "Die Einstellungen wurden erfolgreich gespeichert!",</v>
       </c>
       <c r="H58" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A58,""" : """,D58,""",")</f>
-        <v>"text" : "Denominazione",</v>
+        <v>"settings-stored-success" : "La regulazione è stata salvata di successo!",</v>
       </c>
       <c r="I58" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A58,""" : """,E58,""",")</f>
-        <v>"text" : "Texte",</v>
+        <v>"settings-stored-success" : "Les paramètres ont étés sauvegardés aves succès!",</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="F59" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A59,""" : """,B59,""",")</f>
-        <v>"to" : "to",</v>
+        <v>"show-confirmations" : "Confirmations",</v>
       </c>
       <c r="G59" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A59,""" : """,C59,""",")</f>
-        <v>"to" : "bis",</v>
+        <v>"show-confirmations" : "Bestätigungsmeldungen",</v>
       </c>
       <c r="H59" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A59,""" : """,D59,""",")</f>
-        <v>"to" : "Al",</v>
+        <v>"show-confirmations" : "Confirmazioni",</v>
       </c>
       <c r="I59" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A59,""" : """,E59,""",")</f>
-        <v>"to" : "au",</v>
+        <v>"show-confirmations" : "Confirmations",</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F60" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A60,""" : """,B60,""",")</f>
-        <v>"type" : "Type",</v>
+        <v>"show-notifications" : "Notifications",</v>
       </c>
       <c r="G60" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A60,""" : """,C60,""",")</f>
-        <v>"type" : "Typ",</v>
+        <v>"show-notifications" : "Notifizierungen",</v>
       </c>
       <c r="H60" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A60,""" : """,D60,""",")</f>
-        <v>"type" : "Tipo",</v>
+        <v>"show-notifications" : "Notificazioni",</v>
       </c>
       <c r="I60" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A60,""" : """,E60,""",")</f>
-        <v>"type" : "Type",</v>
+        <v>"show-notifications" : "Notifications",</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>283</v>
       </c>
       <c r="F61" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A61,""" : """,B61,""",")</f>
-        <v>"unlock-card" : "Unlock Card",</v>
+        <v>"start-the-tour" : "Start the tour…",</v>
       </c>
       <c r="G61" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A61,""" : """,C61,""",")</f>
-        <v>"unlock-card" : "Sperrung aufheben",</v>
+        <v>"start-the-tour" : "Beginne die Tour…",</v>
       </c>
       <c r="H61" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A61,""" : """,D61,""",")</f>
-        <v>"unlock-card" : "Sbloccare la carta",</v>
+        <v>"start-the-tour" : "Incomincia il giro…",</v>
       </c>
       <c r="I61" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A61,""" : """,E61,""",")</f>
-        <v>"unlock-card" : "Débloquer la carte",</v>
+        <v>"start-the-tour" : "Commencez le tour…",</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>288</v>
       </c>
       <c r="F62" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A62,""" : """,B62,""",")</f>
-        <v>"valid-from" : "Valid From",</v>
+        <v>"success" : "Success",</v>
       </c>
       <c r="G62" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A62,""" : """,C62,""",")</f>
-        <v>"valid-from" : "Gültig von",</v>
+        <v>"success" : "Erfolg",</v>
       </c>
       <c r="H62" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A62,""" : """,D62,""",")</f>
-        <v>"valid-from" : "Valido dal",</v>
+        <v>"success" : "Successo",</v>
       </c>
       <c r="I62" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A62,""" : """,E62,""",")</f>
-        <v>"valid-from" : "Valable du",</v>
-      </c>
-    </row>
-    <row r="63" s="4" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"success" : "Succès",</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="F63" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A63,""" : """,B63,""",")</f>
-        <v>"version" : "Version",</v>
+        <v>"swipe-through-the-tour-" : "Swipe through the Quick-Tour to get an overview of MX-Banklets' features.",</v>
       </c>
       <c r="G63" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A63,""" : """,C63,""",")</f>
-        <v>"version" : "Version",</v>
+        <v>"swipe-through-the-tour-" : "Wischen Sie durch die Quick-Tour, um einen Überblick über die Features der MX-Banklets zu bekommen. ",</v>
       </c>
       <c r="H63" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A63,""" : """,D63,""",")</f>
-        <v>"version" : "Versione",</v>
+        <v>"swipe-through-the-tour-" : "Passa a traverso il Quick-Tour per ottenere uno sguardo d'insieme delle funzioni die MX-Banklets.",</v>
       </c>
       <c r="I63" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A63,""" : """,E63,""",")</f>
-        <v>"version" : "Version",</v>
-      </c>
-    </row>
-    <row r="64" s="4" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"swipe-through-the-tour-" : "Passez par le Quick-Tour pour ramasser une vue d'ensemble des fonctions des MX-Banklets.",</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="E64" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="F64" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A64,""" : """,B64,""",")</f>
-        <v>"warning" : "Warning",</v>
+        <v>"take-the-tour-" : "Take the Quick-Tour to get an overview of MX-Banklets' features.",</v>
       </c>
       <c r="G64" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A64,""" : """,C64,""",")</f>
-        <v>"warning" : "Achtung",</v>
+        <v>"take-the-tour-" : "Nehmen Sie die Quick-Tour, um einen ersten Überblick über die Features von MX-Banklets zu erhalten.",</v>
       </c>
       <c r="H64" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A64,""" : """,D64,""",")</f>
-        <v>"warning" : "Attenzione",</v>
+        <v>"take-the-tour-" : "Prenda il Quick-Tour per ottenere un primo sguardo sulle funzioni die MX-Banklets.",</v>
       </c>
       <c r="I64" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A64,""" : """,E64,""",")</f>
-        <v>"warning" : "Attention",</v>
-      </c>
-    </row>
-    <row r="65" s="4" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"take-the-tour-" : "Prenez le Quick-Tour pour ramasser une vue d'ensemble des fonctions des MX-Banklets.",</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>298</v>
       </c>
       <c r="F65" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A65,""" : """,B65,""",")</f>
-        <v>"show-confirmations" : "Confirmations",</v>
+        <v>"text" : "Text",</v>
       </c>
       <c r="G65" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A65,""" : """,C65,""",")</f>
-        <v>"show-confirmations" : "Bestätigungsmeldungen",</v>
+        <v>"text" : "Text",</v>
       </c>
       <c r="H65" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A65,""" : """,D65,""",")</f>
-        <v>"show-confirmations" : "Confirmazioni",</v>
+        <v>"text" : "Denominazione",</v>
       </c>
       <c r="I65" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A65,""" : """,E65,""",")</f>
-        <v>"show-confirmations" : "Confirmations",</v>
-      </c>
-    </row>
-    <row r="66" s="4" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"text" : "Texte",</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>302</v>
       </c>
       <c r="F66" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A66,""" : """,B66,""",")</f>
-        <v>"show-notifications" : "Notifications",</v>
+        <v>"to" : "to",</v>
       </c>
       <c r="G66" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A66,""" : """,C66,""",")</f>
-        <v>"show-notifications" : "Notifizierungen",</v>
+        <v>"to" : "bis",</v>
       </c>
       <c r="H66" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A66,""" : """,D66,""",")</f>
-        <v>"show-notifications" : "Notificazioni",</v>
+        <v>"to" : "Al",</v>
       </c>
       <c r="I66" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A66,""" : """,E66,""",")</f>
-        <v>"show-notifications" : "Notifications",</v>
-      </c>
-    </row>
-    <row r="67" s="4" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"to" : "au",</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>309</v>
+      <c r="E67" s="1" t="s">
+        <v>304</v>
       </c>
       <c r="F67" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A67,""" : """,B67,""",")</f>
-        <v>"enter-username-pwd" : "Please enter username 'test' and password 'test'!",</v>
+        <v>"type" : "Type",</v>
       </c>
       <c r="G67" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A67,""" : """,C67,""",")</f>
-        <v>"enter-username-pwd" : "Bitte Benutzername 'test' und Passwort 'test' eingeben!",</v>
+        <v>"type" : "Typ",</v>
       </c>
       <c r="H67" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A67,""" : """,D67,""",")</f>
-        <v>"enter-username-pwd" : "Pregasi immetere il nome dell utente 'test' e la parola d‘accesso 'test'!",</v>
+        <v>"type" : "Tipo",</v>
       </c>
       <c r="I67" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A67,""" : """,E67,""",")</f>
-        <v>"enter-username-pwd" : "Entrez le nom d‘utilisateur 'test' et le mot de passe 'test', s.v.p.!",</v>
-      </c>
-    </row>
-    <row r="68" s="4" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"type" : "Type",</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="E68" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>314</v>
       </c>
       <c r="F68" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A68,""" : """,B68,""",")</f>
-        <v>"start-the-tour" : "Start the tour…",</v>
+        <v>"unlock-card" : "Unlock Card",</v>
       </c>
       <c r="G68" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A68,""" : """,C68,""",")</f>
-        <v>"start-the-tour" : "Beginne die Tour…",</v>
+        <v>"unlock-card" : "Sperrung aufheben",</v>
       </c>
       <c r="H68" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A68,""" : """,D68,""",")</f>
-        <v>"start-the-tour" : "Incomincia il giro…",</v>
+        <v>"unlock-card" : "Sbloccare la carta",</v>
       </c>
       <c r="I68" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A68,""" : """,E68,""",")</f>
-        <v>"start-the-tour" : "Commencez le tour…",</v>
-      </c>
-    </row>
-    <row r="69" s="4" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>"unlock-card" : "Débloquer la carte",</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="E69" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>319</v>
       </c>
       <c r="F69" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A69,""" : """,B69,""",")</f>
@@ -3560,57 +3494,153 @@
         <v>"username" : "Nom d'utilisateur",</v>
       </c>
     </row>
-    <row r="70" s="4" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="E70" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="F70" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A70,""" : """,B70,""",")</f>
-        <v>"yes" : "Yes",</v>
+        <v>"valid-from" : "Valid From",</v>
       </c>
       <c r="G70" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A70,""" : """,C70,""",")</f>
-        <v>"yes" : "Ja",</v>
+        <v>"valid-from" : "Gültig von",</v>
       </c>
       <c r="H70" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A70,""" : """,D70,""",")</f>
-        <v>"yes" : "Sì",</v>
+        <v>"valid-from" : "Valido dal",</v>
       </c>
       <c r="I70" s="1" t="str">
         <f aca="false">CONCATENATE("""",$A70,""" : """,E70,""",")</f>
+        <v>"valid-from" : "Valable du",</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F71" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A71,""" : """,B71,""",")</f>
+        <v>"version" : "Version",</v>
+      </c>
+      <c r="G71" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A71,""" : """,C71,""",")</f>
+        <v>"version" : "Version",</v>
+      </c>
+      <c r="H71" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A71,""" : """,D71,""",")</f>
+        <v>"version" : "Versione",</v>
+      </c>
+      <c r="I71" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A71,""" : """,E71,""",")</f>
+        <v>"version" : "Version",</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F72" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A72,""" : """,B72,""",")</f>
+        <v>"warning" : "Warning",</v>
+      </c>
+      <c r="G72" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A72,""" : """,C72,""",")</f>
+        <v>"warning" : "Achtung",</v>
+      </c>
+      <c r="H72" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A72,""" : """,D72,""",")</f>
+        <v>"warning" : "Attenzione",</v>
+      </c>
+      <c r="I72" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A72,""" : """,E72,""",")</f>
+        <v>"warning" : "Attention",</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F73" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A73,""" : """,B73,""",")</f>
+        <v>"yes" : "Yes",</v>
+      </c>
+      <c r="G73" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A73,""" : """,C73,""",")</f>
+        <v>"yes" : "Ja",</v>
+      </c>
+      <c r="H73" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A73,""" : """,D73,""",")</f>
+        <v>"yes" : "Sì",</v>
+      </c>
+      <c r="I73" s="1" t="str">
+        <f aca="false">CONCATENATE("""",$A73,""" : """,E73,""",")</f>
         <v>"yes" : "Oui",</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F71" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="72" s="5" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F74" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="75" s="5" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>